<commit_message>
Reference mail RE: rd_deal STM issue
please change to decimal(4,1)
</commit_message>
<xml_diff>
--- a/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V0.9.xlsx
+++ b/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V0.9.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8114" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8114" uniqueCount="602">
   <si>
     <t>Mode of Integration</t>
   </si>
@@ -1864,6 +1864,9 @@
   </si>
   <si>
     <t>TAC_PROP</t>
+  </si>
+  <si>
+    <t>DECIMAL(4,1)</t>
   </si>
 </sst>
 </file>
@@ -2992,13 +2995,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="29" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="29" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
@@ -3034,20 +3051,6 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3357,12 +3360,12 @@
       <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="20.25">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="165" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="20"/>
@@ -3386,10 +3389,10 @@
       <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="166" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="161"/>
+      <c r="B8" s="167"/>
       <c r="C8" s="27" t="s">
         <v>63</v>
       </c>
@@ -3416,7 +3419,7 @@
       <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="168" t="s">
         <v>69</v>
       </c>
       <c r="B10" s="31" t="s">
@@ -3428,7 +3431,7 @@
       <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="163"/>
+      <c r="A11" s="169"/>
       <c r="B11" s="37" t="s">
         <v>71</v>
       </c>
@@ -3458,7 +3461,7 @@
       <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="15.75">
-      <c r="A14" s="164" t="s">
+      <c r="A14" s="170" t="s">
         <v>74</v>
       </c>
       <c r="B14" s="37" t="s">
@@ -3470,7 +3473,7 @@
       <c r="F14" s="41"/>
     </row>
     <row r="15" spans="1:6" ht="15.75">
-      <c r="A15" s="165"/>
+      <c r="A15" s="171"/>
       <c r="B15" s="31" t="s">
         <v>73</v>
       </c>
@@ -3480,7 +3483,7 @@
       <c r="F15" s="44"/>
     </row>
     <row r="16" spans="1:6" ht="15.75">
-      <c r="A16" s="165"/>
+      <c r="A16" s="171"/>
       <c r="B16" s="31" t="s">
         <v>76</v>
       </c>
@@ -3490,7 +3493,7 @@
       <c r="F16" s="44"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A17" s="166"/>
+      <c r="A17" s="172"/>
       <c r="B17" s="46" t="s">
         <v>77</v>
       </c>
@@ -3527,11 +3530,11 @@
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="167" t="s">
+      <c r="D20" s="173" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="168"/>
-      <c r="F20" s="169"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="175"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1">
       <c r="A21" s="54">
@@ -3543,11 +3546,11 @@
       <c r="C21" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="156" t="s">
+      <c r="D21" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="157"/>
-      <c r="F21" s="158"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="163"/>
     </row>
     <row r="22" spans="1:6" ht="36.75" customHeight="1">
       <c r="A22" s="57">
@@ -3559,11 +3562,11 @@
       <c r="C22" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="171" t="s">
+      <c r="D22" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="171"/>
-      <c r="F22" s="172"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="160"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" customHeight="1">
       <c r="A23" s="57">
@@ -3575,11 +3578,11 @@
       <c r="C23" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="171" t="s">
+      <c r="D23" s="159" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="171"/>
-      <c r="F23" s="172"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="160"/>
     </row>
     <row r="24" spans="1:6" ht="44.25" customHeight="1">
       <c r="A24" s="57">
@@ -3591,11 +3594,11 @@
       <c r="C24" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="171" t="s">
+      <c r="D24" s="159" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="171"/>
-      <c r="F24" s="172"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="160"/>
     </row>
     <row r="25" spans="1:6" ht="89.25" customHeight="1">
       <c r="A25" s="57">
@@ -3607,11 +3610,11 @@
       <c r="C25" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="173" t="s">
+      <c r="D25" s="161" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="157"/>
-      <c r="F25" s="158"/>
+      <c r="E25" s="162"/>
+      <c r="F25" s="163"/>
     </row>
     <row r="26" spans="1:6" ht="44.25" customHeight="1">
       <c r="A26" s="57">
@@ -3623,11 +3626,11 @@
       <c r="C26" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="170" t="s">
+      <c r="D26" s="158" t="s">
         <v>579</v>
       </c>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
+      <c r="E26" s="158"/>
+      <c r="F26" s="158"/>
     </row>
     <row r="27" spans="1:6" ht="44.25" customHeight="1">
       <c r="A27" s="57">
@@ -3639,26 +3642,26 @@
       <c r="C27" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="170" t="s">
+      <c r="D27" s="158" t="s">
         <v>580</v>
       </c>
-      <c r="E27" s="170"/>
-      <c r="F27" s="170"/>
+      <c r="E27" s="158"/>
+      <c r="F27" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10146,9 +10149,9 @@
   </sheetPr>
   <dimension ref="A1:X676"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -10303,13 +10306,13 @@
       <c r="B3" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="175" t="s">
+      <c r="C3" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D3" s="87" t="s">
         <v>262</v>
       </c>
-      <c r="E3" s="174"/>
+      <c r="E3" s="156"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14" t="s">
@@ -10347,13 +10350,13 @@
       <c r="B4" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="175" t="s">
+      <c r="C4" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D4" s="87" t="s">
         <v>264</v>
       </c>
-      <c r="E4" s="174"/>
+      <c r="E4" s="156"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14" t="s">
@@ -10391,13 +10394,13 @@
       <c r="B5" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C5" s="175" t="s">
+      <c r="C5" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D5" s="87" t="s">
         <v>266</v>
       </c>
-      <c r="E5" s="174"/>
+      <c r="E5" s="156"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
@@ -10435,13 +10438,13 @@
       <c r="B6" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C6" s="175" t="s">
+      <c r="C6" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D6" s="87" t="s">
         <v>267</v>
       </c>
-      <c r="E6" s="174"/>
+      <c r="E6" s="156"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14" t="s">
@@ -10479,13 +10482,13 @@
       <c r="B7" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C7" s="175" t="s">
+      <c r="C7" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D7" s="87" t="s">
         <v>269</v>
       </c>
-      <c r="E7" s="174"/>
+      <c r="E7" s="156"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
@@ -10523,13 +10526,13 @@
       <c r="B8" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C8" s="175" t="s">
+      <c r="C8" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D8" s="87" t="s">
         <v>270</v>
       </c>
-      <c r="E8" s="174"/>
+      <c r="E8" s="156"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
@@ -10571,13 +10574,13 @@
       <c r="B9" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="175" t="s">
+      <c r="C9" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D9" s="87" t="s">
         <v>272</v>
       </c>
-      <c r="E9" s="174"/>
+      <c r="E9" s="156"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
@@ -10619,13 +10622,13 @@
       <c r="B10" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="175" t="s">
+      <c r="C10" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D10" s="87" t="s">
         <v>273</v>
       </c>
-      <c r="E10" s="174"/>
+      <c r="E10" s="156"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
@@ -10663,13 +10666,13 @@
       <c r="B11" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C11" s="175" t="s">
+      <c r="C11" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D11" s="87" t="s">
         <v>275</v>
       </c>
-      <c r="E11" s="174"/>
+      <c r="E11" s="156"/>
       <c r="F11" s="77"/>
       <c r="G11" s="77"/>
       <c r="H11" s="14" t="s">
@@ -10707,13 +10710,13 @@
       <c r="B12" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="175" t="s">
+      <c r="C12" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D12" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="E12" s="174"/>
+      <c r="E12" s="156"/>
       <c r="F12" s="77"/>
       <c r="G12" s="77"/>
       <c r="H12" s="14" t="s">
@@ -10751,13 +10754,13 @@
       <c r="B13" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C13" s="175" t="s">
+      <c r="C13" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D13" s="87" t="s">
         <v>277</v>
       </c>
-      <c r="E13" s="174"/>
+      <c r="E13" s="156"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
@@ -10795,13 +10798,13 @@
       <c r="B14" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C14" s="175" t="s">
+      <c r="C14" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D14" s="87" t="s">
         <v>279</v>
       </c>
-      <c r="E14" s="174"/>
+      <c r="E14" s="156"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
@@ -10843,13 +10846,13 @@
       <c r="B15" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C15" s="175" t="s">
+      <c r="C15" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D15" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="E15" s="174"/>
+      <c r="E15" s="156"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14" t="s">
@@ -10891,13 +10894,13 @@
       <c r="B16" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C16" s="175" t="s">
+      <c r="C16" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D16" s="87" t="s">
         <v>282</v>
       </c>
-      <c r="E16" s="174"/>
+      <c r="E16" s="156"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14" t="s">
@@ -10939,13 +10942,13 @@
       <c r="B17" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C17" s="175" t="s">
+      <c r="C17" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D17" s="87" t="s">
         <v>284</v>
       </c>
-      <c r="E17" s="174"/>
+      <c r="E17" s="156"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14" t="s">
@@ -10987,13 +10990,13 @@
       <c r="B18" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C18" s="175" t="s">
+      <c r="C18" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D18" s="87" t="s">
         <v>285</v>
       </c>
-      <c r="E18" s="174" t="s">
+      <c r="E18" s="156" t="s">
         <v>298</v>
       </c>
       <c r="F18" s="14"/>
@@ -11035,13 +11038,13 @@
       <c r="B19" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C19" s="175" t="s">
+      <c r="C19" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D19" s="87" t="s">
         <v>286</v>
       </c>
-      <c r="E19" s="174" t="s">
+      <c r="E19" s="156" t="s">
         <v>298</v>
       </c>
       <c r="F19" s="14"/>
@@ -11083,13 +11086,13 @@
       <c r="B20" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C20" s="175" t="s">
+      <c r="C20" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D20" s="87" t="s">
         <v>287</v>
       </c>
-      <c r="E20" s="174"/>
+      <c r="E20" s="156"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14" t="s">
@@ -11127,13 +11130,13 @@
       <c r="B21" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C21" s="175" t="s">
+      <c r="C21" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D21" s="87" t="s">
         <v>289</v>
       </c>
-      <c r="E21" s="174"/>
+      <c r="E21" s="156"/>
       <c r="F21" s="77"/>
       <c r="G21" s="77"/>
       <c r="H21" s="14" t="s">
@@ -11171,13 +11174,13 @@
       <c r="B22" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C22" s="175" t="s">
+      <c r="C22" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D22" s="87" t="s">
         <v>290</v>
       </c>
-      <c r="E22" s="174"/>
+      <c r="E22" s="156"/>
       <c r="F22" s="77"/>
       <c r="G22" s="77"/>
       <c r="H22" s="14" t="s">
@@ -11215,13 +11218,13 @@
       <c r="B23" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C23" s="175" t="s">
+      <c r="C23" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D23" s="87" t="s">
         <v>292</v>
       </c>
-      <c r="E23" s="174" t="s">
+      <c r="E23" s="156" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="14"/>
@@ -11263,13 +11266,13 @@
       <c r="B24" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C24" s="175" t="s">
+      <c r="C24" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D24" s="87" t="s">
         <v>293</v>
       </c>
-      <c r="E24" s="174"/>
+      <c r="E24" s="156"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14" t="s">
@@ -11307,13 +11310,13 @@
       <c r="B25" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C25" s="175" t="s">
+      <c r="C25" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D25" s="87" t="s">
         <v>295</v>
       </c>
-      <c r="E25" s="174" t="s">
+      <c r="E25" s="156" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="14"/>
@@ -11355,13 +11358,13 @@
       <c r="B26" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C26" s="175" t="s">
+      <c r="C26" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D26" s="87" t="s">
         <v>296</v>
       </c>
-      <c r="E26" s="174"/>
+      <c r="E26" s="156"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14" t="s">
@@ -11399,13 +11402,13 @@
       <c r="B27" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C27" s="175" t="s">
+      <c r="C27" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D27" s="87" t="s">
         <v>596</v>
       </c>
-      <c r="E27" s="174"/>
+      <c r="E27" s="156"/>
       <c r="F27" s="112"/>
       <c r="G27" s="112"/>
       <c r="H27" s="14" t="s">
@@ -11443,13 +11446,13 @@
       <c r="B28" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C28" s="175" t="s">
+      <c r="C28" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D28" s="87" t="s">
         <v>597</v>
       </c>
-      <c r="E28" s="174"/>
+      <c r="E28" s="156"/>
       <c r="F28" s="112"/>
       <c r="G28" s="112"/>
       <c r="H28" s="14" t="s">
@@ -11487,13 +11490,13 @@
       <c r="B29" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C29" s="175" t="s">
+      <c r="C29" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D29" s="87" t="s">
         <v>598</v>
       </c>
-      <c r="E29" s="174"/>
+      <c r="E29" s="156"/>
       <c r="F29" s="112"/>
       <c r="G29" s="112"/>
       <c r="H29" s="14" t="s">
@@ -11531,13 +11534,13 @@
       <c r="B30" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C30" s="175" t="s">
+      <c r="C30" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D30" s="87" t="s">
         <v>599</v>
       </c>
-      <c r="E30" s="174"/>
+      <c r="E30" s="156"/>
       <c r="F30" s="112"/>
       <c r="G30" s="112"/>
       <c r="H30" s="14" t="s">
@@ -11575,13 +11578,13 @@
       <c r="B31" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="175" t="s">
+      <c r="C31" s="157" t="s">
         <v>261</v>
       </c>
       <c r="D31" s="87" t="s">
         <v>600</v>
       </c>
-      <c r="E31" s="174"/>
+      <c r="E31" s="156"/>
       <c r="F31" s="112"/>
       <c r="G31" s="112"/>
       <c r="H31" s="14" t="s">
@@ -19109,7 +19112,7 @@
         <v>375</v>
       </c>
       <c r="J205" s="87" t="s">
-        <v>376</v>
+        <v>601</v>
       </c>
       <c r="K205" s="87" t="s">
         <v>376</v>
@@ -40566,18 +40569,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40600,14 +40603,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C16B0E6-E226-461B-8D00-37FDE1E9DF80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70785B63-45C8-4C04-9C8C-D6290BDFADA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -40622,4 +40617,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C16B0E6-E226-461B-8D00-37FDE1E9DF80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>